<commit_message>
Fix bugs found while presenting :)
</commit_message>
<xml_diff>
--- a/src/assets/images/nmf/NMF_factorization.xlsx
+++ b/src/assets/images/nmf/NMF_factorization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beni/IdeaProjects/cas-machine-learning-slides/src/assets/images/nmf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5911D1-ABA7-1742-814B-93A6708B3260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0F03FC-602C-6044-9C88-E4AFE7438BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{1FEFB6AC-59FD-0B43-AD12-C022DB4FB7A3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{1FEFB6AC-59FD-0B43-AD12-C022DB4FB7A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -114,6 +114,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,7 +436,7 @@
   <dimension ref="B5:X17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,9 +465,9 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
     </row>
     <row r="8" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
@@ -477,9 +481,9 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
     </row>
     <row r="9" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
@@ -493,9 +497,9 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
@@ -536,9 +540,9 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
     </row>
     <row r="14" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
@@ -557,9 +561,9 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
     </row>
     <row r="15" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
@@ -596,8 +600,8 @@
     <mergeCell ref="G13:I15"/>
     <mergeCell ref="N13:P15"/>
     <mergeCell ref="K7:L9"/>
-    <mergeCell ref="R7:X9"/>
     <mergeCell ref="B7:E9"/>
+    <mergeCell ref="R7:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>